<commit_message>
Automation Practice test by BrainStation23 with Report
</commit_message>
<xml_diff>
--- a/src/test/java/com/DataDriven/Login_data.xlsx
+++ b/src/test/java/com/DataDriven/Login_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Apps\Java\IntelliJ\AutomationWithJavaPnT\src\test\java\com\DataDriven\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>Email</t>
   </si>
@@ -55,12 +55,16 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>Didn't login, Test passed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -397,9 +401,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.77734375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="23.77734375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.77734375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="19.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -423,6 +427,9 @@
       <c r="B2">
         <v>123456</v>
       </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -431,6 +438,9 @@
       <c r="B3">
         <v>123456</v>
       </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -439,6 +449,9 @@
       <c r="B4">
         <v>123456</v>
       </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -447,6 +460,9 @@
       <c r="B5">
         <v>123456</v>
       </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -455,6 +471,9 @@
       <c r="B6">
         <v>123456</v>
       </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -462,6 +481,9 @@
       </c>
       <c r="B7">
         <v>123456</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>